<commit_message>
User - Drafts contains more info about town
</commit_message>
<xml_diff>
--- a/data_sheets/towns.xlsx
+++ b/data_sheets/towns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\tubemaphistory\tube-map-history.api\data_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0312F6-90FD-42D5-9DCE-B8E68E52C7DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D4C2CB-E79F-41A0-8076-31D4FD897BA6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-4356" windowWidth="30936" windowHeight="16896" xr2:uid="{6A4D07FD-A3BF-472B-A872-BFD1BF1F63B5}"/>
+    <workbookView xWindow="24576" yWindow="-2712" windowWidth="23040" windowHeight="12204" xr2:uid="{6A4D07FD-A3BF-472B-A872-BFD1BF1F63B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Towns" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>name</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>order</t>
   </si>
 </sst>
 </file>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D28E414-4E16-4B41-99B9-DFDB36752E79}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,7 +548,7 @@
     <col min="5" max="5" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,8 +573,11 @@
       <c r="H1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -596,8 +602,11 @@
       <c r="H2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -622,8 +631,11 @@
       <c r="H3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -648,8 +660,11 @@
       <c r="H4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -674,8 +689,11 @@
       <c r="H5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -700,8 +718,11 @@
       <c r="H6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -726,8 +747,11 @@
       <c r="H7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -752,8 +776,11 @@
       <c r="H8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -778,8 +805,11 @@
       <c r="H9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -804,8 +834,11 @@
       <c r="H10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -830,8 +863,11 @@
       <c r="H11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -856,8 +892,11 @@
       <c r="H12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -882,8 +921,11 @@
       <c r="H13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -907,6 +949,9 @@
       </c>
       <c r="H14" t="s">
         <v>23</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>